<commit_message>
Hotfix: updated DALY defaults in framework and demo project
Changed "key calibration parameters" to "key calibration estimates" to
minimize confusion.

Added defaults and guidance for DALYs
</commit_message>
<xml_diff>
--- a/atomica_apps/optima_tb_databook.xlsx
+++ b/atomica_apps/optima_tb_databook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Latent treatment" sheetId="5" r:id="rId5"/>
     <sheet name="Initialization estimates" sheetId="6" r:id="rId6"/>
     <sheet name="New infections proportions" sheetId="7" r:id="rId7"/>
-    <sheet name="Key calibration parameters" sheetId="8" r:id="rId8"/>
+    <sheet name="Key calibration estimates" sheetId="8" r:id="rId8"/>
     <sheet name="Optional data" sheetId="9" r:id="rId9"/>
     <sheet name="Infection susceptibility" sheetId="10" r:id="rId10"/>
     <sheet name="Untreated TB progression rates" sheetId="11" r:id="rId11"/>
@@ -2954,18 +2954,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
@@ -5060,6 +5048,18 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor rgb="FF98E0FA"/>
         </patternFill>
@@ -6975,7 +6975,7 @@
   <dimension ref="A1:X48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8839,7 +8839,7 @@
   <dimension ref="A1:X118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13305,8 +13305,8 @@
   </sheetPr>
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13399,9 +13399,11 @@
       <c r="B2" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3">
+        <v>0.111</v>
+      </c>
       <c r="D2" s="3">
-        <v>1</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>18</v>
@@ -13434,9 +13436,11 @@
       <c r="B3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <v>0.111</v>
+      </c>
       <c r="D3" s="3">
-        <v>1</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>18</v>
@@ -13469,9 +13473,11 @@
       <c r="B4" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>0.111</v>
+      </c>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>18</v>
@@ -13504,9 +13510,11 @@
       <c r="B5" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>0.111</v>
+      </c>
       <c r="D5" s="3">
-        <v>1</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>18</v>
@@ -13539,9 +13547,11 @@
       <c r="B6" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>0.111</v>
+      </c>
       <c r="D6" s="3">
-        <v>1</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>18</v>
@@ -13648,7 +13658,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>18</v>
@@ -13683,7 +13693,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>18</v>
@@ -13753,7 +13763,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>18</v>
@@ -13814,7 +13824,7 @@
       <c r="X13" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6 D9:D13">
+  <conditionalFormatting sqref="D9:D13 D2:D6">
     <cfRule type="expression" dxfId="240" priority="319">
       <formula>COUNTIF(F2:X2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
@@ -13842,7 +13852,7 @@
   </sheetPr>
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -15512,10 +15522,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F36">
-    <cfRule type="expression" dxfId="1" priority="387">
+    <cfRule type="expression" dxfId="163" priority="387">
       <formula>COUNTIF(H12:Z12,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="388">
+    <cfRule type="expression" dxfId="162" priority="388">
       <formula>AND(COUNTIF(H12:Z12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F12)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18071,694 +18081,694 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="163" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="154" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="155" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="161" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="162" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="163" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="159" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="170" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="171" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="157" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="178" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="179" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="155" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="39" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="40" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="153" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="47" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="48" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="151" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="55" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="56" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="149" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="63" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="64" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="147" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="146" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="147" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="145" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="164" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="165" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="cellIs" dxfId="143" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="172" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="173" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="141" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="180" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="181" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="139" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="31" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="32" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="137" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="49" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="50" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="135" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="57" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="58" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="133" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="65" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="66" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:Z12">
-    <cfRule type="expression" dxfId="131" priority="73">
+    <cfRule type="expression" dxfId="129" priority="73">
       <formula>$B$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:G13 S13:Z13">
-    <cfRule type="expression" dxfId="130" priority="76">
+    <cfRule type="expression" dxfId="128" priority="76">
       <formula>$C$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:Z14">
-    <cfRule type="expression" dxfId="129" priority="79">
+    <cfRule type="expression" dxfId="127" priority="79">
       <formula>$D$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:Z15">
-    <cfRule type="expression" dxfId="128" priority="82">
+    <cfRule type="expression" dxfId="126" priority="82">
       <formula>$E$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:Z16">
-    <cfRule type="expression" dxfId="127" priority="85">
+    <cfRule type="expression" dxfId="125" priority="85">
       <formula>$F$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:Z17">
-    <cfRule type="expression" dxfId="126" priority="88">
+    <cfRule type="expression" dxfId="124" priority="88">
       <formula>$B$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:Z18">
-    <cfRule type="expression" dxfId="125" priority="91">
+    <cfRule type="expression" dxfId="123" priority="91">
       <formula>$C$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:G19 X19:Z19">
-    <cfRule type="expression" dxfId="124" priority="94">
+    <cfRule type="expression" dxfId="122" priority="94">
       <formula>$D$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:Z20">
-    <cfRule type="expression" dxfId="123" priority="97">
+    <cfRule type="expression" dxfId="121" priority="97">
       <formula>$E$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:Z21">
-    <cfRule type="expression" dxfId="122" priority="100">
+    <cfRule type="expression" dxfId="120" priority="100">
       <formula>$F$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:Z22">
-    <cfRule type="expression" dxfId="121" priority="103">
+    <cfRule type="expression" dxfId="119" priority="103">
       <formula>$B$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:Z23">
-    <cfRule type="expression" dxfId="120" priority="106">
+    <cfRule type="expression" dxfId="118" priority="106">
       <formula>$C$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:Z24">
-    <cfRule type="expression" dxfId="119" priority="109">
+    <cfRule type="expression" dxfId="117" priority="109">
       <formula>$D$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:G25 X25:Z25">
-    <cfRule type="expression" dxfId="118" priority="112">
+    <cfRule type="expression" dxfId="116" priority="112">
       <formula>$E$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:Z26">
-    <cfRule type="expression" dxfId="117" priority="115">
+    <cfRule type="expression" dxfId="115" priority="115">
       <formula>$F$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:Z27">
-    <cfRule type="expression" dxfId="116" priority="118">
+    <cfRule type="expression" dxfId="114" priority="118">
       <formula>$B$8&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:Z28">
-    <cfRule type="expression" dxfId="115" priority="121">
+    <cfRule type="expression" dxfId="113" priority="121">
       <formula>$C$8&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:Z29">
-    <cfRule type="expression" dxfId="114" priority="124">
+    <cfRule type="expression" dxfId="112" priority="124">
       <formula>$D$8&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:Z30">
-    <cfRule type="expression" dxfId="113" priority="127">
+    <cfRule type="expression" dxfId="111" priority="127">
       <formula>$E$8&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:Z31">
-    <cfRule type="expression" dxfId="112" priority="130">
+    <cfRule type="expression" dxfId="110" priority="130">
       <formula>$F$8&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:Z32">
-    <cfRule type="expression" dxfId="111" priority="133">
+    <cfRule type="expression" dxfId="109" priority="133">
       <formula>$B$9&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:Z33">
-    <cfRule type="expression" dxfId="110" priority="136">
+    <cfRule type="expression" dxfId="108" priority="136">
       <formula>$C$9&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:Z34">
-    <cfRule type="expression" dxfId="109" priority="139">
+    <cfRule type="expression" dxfId="107" priority="139">
       <formula>$D$9&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:Z35">
-    <cfRule type="expression" dxfId="108" priority="142">
+    <cfRule type="expression" dxfId="106" priority="142">
       <formula>$E$9&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:Z36">
-    <cfRule type="expression" dxfId="107" priority="145">
+    <cfRule type="expression" dxfId="105" priority="145">
       <formula>$F$9&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="cellIs" dxfId="106" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="148" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="149" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="104" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="156" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="157" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="102" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="174" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="175" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="100" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="182" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="183" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:Z49">
-    <cfRule type="expression" dxfId="98" priority="188">
+    <cfRule type="expression" dxfId="96" priority="188">
       <formula>$B$42&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="97" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="33" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="34" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50:Z50">
-    <cfRule type="expression" dxfId="95" priority="191">
+    <cfRule type="expression" dxfId="93" priority="191">
       <formula>$C$42&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:Z51">
-    <cfRule type="expression" dxfId="94" priority="194">
+    <cfRule type="expression" dxfId="92" priority="194">
       <formula>$D$42&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:Z52">
-    <cfRule type="expression" dxfId="93" priority="197">
+    <cfRule type="expression" dxfId="91" priority="197">
       <formula>$E$42&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53:Z53">
-    <cfRule type="expression" dxfId="92" priority="200">
+    <cfRule type="expression" dxfId="90" priority="200">
       <formula>$F$42&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54:Z54">
-    <cfRule type="expression" dxfId="91" priority="203">
+    <cfRule type="expression" dxfId="89" priority="203">
       <formula>$B$43&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:Z55">
-    <cfRule type="expression" dxfId="90" priority="206">
+    <cfRule type="expression" dxfId="88" priority="206">
       <formula>$C$43&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56:Z56">
-    <cfRule type="expression" dxfId="89" priority="209">
+    <cfRule type="expression" dxfId="87" priority="209">
       <formula>$D$43&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:Z57">
-    <cfRule type="expression" dxfId="88" priority="212">
+    <cfRule type="expression" dxfId="86" priority="212">
       <formula>$E$43&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58:Z58">
-    <cfRule type="expression" dxfId="87" priority="215">
+    <cfRule type="expression" dxfId="85" priority="215">
       <formula>$F$43&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59:Z59">
-    <cfRule type="expression" dxfId="86" priority="218">
+    <cfRule type="expression" dxfId="84" priority="218">
       <formula>$B$44&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="85" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="41" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="42" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60:Z60">
-    <cfRule type="expression" dxfId="83" priority="221">
+    <cfRule type="expression" dxfId="81" priority="221">
       <formula>$C$44&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61:Z61">
-    <cfRule type="expression" dxfId="82" priority="224">
+    <cfRule type="expression" dxfId="80" priority="224">
       <formula>$D$44&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:Z62">
-    <cfRule type="expression" dxfId="81" priority="227">
+    <cfRule type="expression" dxfId="79" priority="227">
       <formula>$E$44&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:E63 G63:Z63">
-    <cfRule type="expression" dxfId="80" priority="230">
+    <cfRule type="expression" dxfId="78" priority="230">
       <formula>$F$44&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:E64 G64:Z64">
-    <cfRule type="expression" dxfId="79" priority="233">
+    <cfRule type="expression" dxfId="77" priority="233">
       <formula>$B$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:E65 G65:Z65">
-    <cfRule type="expression" dxfId="78" priority="236">
+    <cfRule type="expression" dxfId="76" priority="236">
       <formula>$C$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:E66 G66:Z66">
-    <cfRule type="expression" dxfId="77" priority="239">
+    <cfRule type="expression" dxfId="75" priority="239">
       <formula>$D$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67:E67 G67:Z67">
-    <cfRule type="expression" dxfId="76" priority="242">
+    <cfRule type="expression" dxfId="74" priority="242">
       <formula>$E$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68:E68 G68:Z68">
-    <cfRule type="expression" dxfId="75" priority="245">
+    <cfRule type="expression" dxfId="73" priority="245">
       <formula>$F$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:E69 G69:Z69">
-    <cfRule type="expression" dxfId="74" priority="248">
+    <cfRule type="expression" dxfId="72" priority="248">
       <formula>$B$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70:E70 G70:Z70">
-    <cfRule type="expression" dxfId="73" priority="251">
+    <cfRule type="expression" dxfId="71" priority="251">
       <formula>$C$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:E71 G71:Z71">
-    <cfRule type="expression" dxfId="72" priority="254">
+    <cfRule type="expression" dxfId="70" priority="254">
       <formula>$D$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72:Z72">
-    <cfRule type="expression" dxfId="71" priority="257">
+    <cfRule type="expression" dxfId="69" priority="257">
       <formula>$E$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73:Z73">
-    <cfRule type="expression" dxfId="70" priority="260">
+    <cfRule type="expression" dxfId="68" priority="260">
       <formula>$F$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="69" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="60" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="65" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="150" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="151" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="63" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="158" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="159" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="61" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="166" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="167" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="59" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="184" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="185" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="57" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="35" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="36" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="55" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="44" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="51" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="69" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="70" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="cellIs" dxfId="49" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="152" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="153" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="cellIs" dxfId="47" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="160" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="161" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44">
-    <cfRule type="cellIs" dxfId="45" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="168" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="169" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45">
-    <cfRule type="cellIs" dxfId="43" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="176" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="177" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="41" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="37" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="53" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="54" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="35" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="61" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="62" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:R13">
-    <cfRule type="expression" dxfId="33" priority="30">
+    <cfRule type="expression" dxfId="31" priority="30">
       <formula>$C$5&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:W19">
-    <cfRule type="expression" dxfId="32" priority="29">
+    <cfRule type="expression" dxfId="30" priority="29">
       <formula>$D$6&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:W25">
-    <cfRule type="expression" dxfId="31" priority="28">
+    <cfRule type="expression" dxfId="29" priority="28">
       <formula>$E$7&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63">
-    <cfRule type="expression" dxfId="30" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>COUNTIF(H63:Y63,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>AND(COUNTIF(H63:Y63,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F63)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="26" priority="3">
       <formula>$F$44&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="27" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>COUNTIF(H64:Y64,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="5">
+    <cfRule type="expression" dxfId="24" priority="5">
       <formula>AND(COUNTIF(H64:Y64,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F64)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="6">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>$B$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65">
-    <cfRule type="expression" dxfId="24" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>COUNTIF(H65:Y65,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="8">
+    <cfRule type="expression" dxfId="21" priority="8">
       <formula>AND(COUNTIF(H65:Y65,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F65)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="20" priority="9">
       <formula>$C$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="expression" dxfId="21" priority="10">
+    <cfRule type="expression" dxfId="19" priority="10">
       <formula>COUNTIF(H66:Y66,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="11">
+    <cfRule type="expression" dxfId="18" priority="11">
       <formula>AND(COUNTIF(H66:Y66,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F66)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="12">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>$D$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67">
-    <cfRule type="expression" dxfId="18" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>COUNTIF(H67:Y67,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="14">
+    <cfRule type="expression" dxfId="15" priority="14">
       <formula>AND(COUNTIF(H67:Y67,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F67)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$E$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F68">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>COUNTIF(H68:Y68,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17">
+    <cfRule type="expression" dxfId="12" priority="17">
       <formula>AND(COUNTIF(H68:Y68,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F68)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="18">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>$F$45&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69">
-    <cfRule type="expression" dxfId="12" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>COUNTIF(H69:Y69,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20">
+    <cfRule type="expression" dxfId="9" priority="20">
       <formula>AND(COUNTIF(H69:Y69,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F69)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="21">
+    <cfRule type="expression" dxfId="8" priority="21">
       <formula>$B$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="7" priority="22">
       <formula>COUNTIF(H70:Y70,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="23">
+    <cfRule type="expression" dxfId="6" priority="23">
       <formula>AND(COUNTIF(H70:Y70,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F70)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="24">
+    <cfRule type="expression" dxfId="5" priority="24">
       <formula>$C$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="6" priority="25">
+    <cfRule type="expression" dxfId="4" priority="25">
       <formula>COUNTIF(H71:Y71,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="26">
+    <cfRule type="expression" dxfId="3" priority="26">
       <formula>AND(COUNTIF(H71:Y71,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F71)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="27">
+    <cfRule type="expression" dxfId="2" priority="27">
       <formula>$D$46&lt;&gt;"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F36 F49:F62 F72:F73">
-    <cfRule type="expression" dxfId="3" priority="321">
+    <cfRule type="expression" dxfId="1" priority="321">
       <formula>COUNTIF(H12:Z12,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="322">
+    <cfRule type="expression" dxfId="0" priority="322">
       <formula>AND(COUNTIF(H12:Z12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(F12)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18826,7 +18836,7 @@
   </sheetPr>
   <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -37987,11 +37997,11 @@
   </sheetPr>
   <dimension ref="A1:X135"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="I102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L67" sqref="L67"/>
+      <selection pane="bottomRight" activeCell="Q136" sqref="Q136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42952,8 +42962,8 @@
   </sheetPr>
   <dimension ref="A1:X214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50608,6 +50618,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>